<commit_message>
Last set of test fixes and clean-up.
- There was an oversight on buffer cleanup I found when the AggregatedErrors is raised.  Added a clear_update_buffer() call.
- Reverted get_researchers() to supply the tracebase database, because that allows the tests to work as designed.  This will of course eventually go away as a part of this effort.
- Reverted tests that were changed because of the above reversion

Files checked in: DataRepo/example_data/data_submission_accucor1.xlsx DataRepo/example_data/data_submission_accucor2.xlsx DataRepo/example_data/data_submission_animal_sample_table.xlsx DataRepo/models/maintained_model.py DataRepo/tests/models/test_animal.py DataRepo/tests/models/test_hier_cached_model.py DataRepo/tests/test_formats.py DataRepo/tests/test_models.py DataRepo/tests/test_views.py DataRepo/tests/views/test_home_views.py DataRepo/tests/views/test_protocol_views.py DataRepo/utils/sample_table_loader.py DataRepo/views/loading/validation.py
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/data_submission_accucor1.xlsx
+++ b/DataRepo/example_data/data_submission_accucor1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mjm12/Desktop/TraceBase Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0259B205-14B5-D24A-A076-053F2D2A7101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{061EEBC0-7B67-8646-8FAB-FF18B044CC4E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1360" windowWidth="26760" windowHeight="9960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1360" windowWidth="44960" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Normalized" sheetId="3" r:id="rId3"/>
     <sheet name="PoolAfterDF" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -76,51 +76,6 @@
     <t>blank_404020_15N_AAmix_1Xstd</t>
   </si>
   <si>
-    <t>M1_1_TS1</t>
-  </si>
-  <si>
-    <t>M1_2_bra</t>
-  </si>
-  <si>
-    <t>M1_3_quad</t>
-  </si>
-  <si>
-    <t>M1_4_kid</t>
-  </si>
-  <si>
-    <t>M1_5_liv</t>
-  </si>
-  <si>
-    <t>M1_6_spl</t>
-  </si>
-  <si>
-    <t>M1_7_panc</t>
-  </si>
-  <si>
-    <t>M1_8_stom</t>
-  </si>
-  <si>
-    <t>M1_9_lung</t>
-  </si>
-  <si>
-    <t>M1_10_hea</t>
-  </si>
-  <si>
-    <t>M1_11_thy</t>
-  </si>
-  <si>
-    <t>M1_12_gWAT</t>
-  </si>
-  <si>
-    <t>M1_13_iBAT</t>
-  </si>
-  <si>
-    <t>M1_14_SI</t>
-  </si>
-  <si>
-    <t>M1_15_ears</t>
-  </si>
-  <si>
     <t>C12 PARENT</t>
   </si>
   <si>
@@ -164,6 +119,51 @@
   </si>
   <si>
     <t>C_Label</t>
+  </si>
+  <si>
+    <t>072920_XXX1_1_TS1</t>
+  </si>
+  <si>
+    <t>072920_XXX1_2_bra</t>
+  </si>
+  <si>
+    <t>072920_XXX1_3_quad</t>
+  </si>
+  <si>
+    <t>072920_XXX1_4_kid</t>
+  </si>
+  <si>
+    <t>072920_XXX1_5_liv</t>
+  </si>
+  <si>
+    <t>072920_XXX1_6_spl</t>
+  </si>
+  <si>
+    <t>072920_XXX1_7_panc</t>
+  </si>
+  <si>
+    <t>072920_XXX1_8_stom</t>
+  </si>
+  <si>
+    <t>072920_XXX1_9_lung</t>
+  </si>
+  <si>
+    <t>072920_XXX1_10_hea</t>
+  </si>
+  <si>
+    <t>072920_XXX1_11_thy</t>
+  </si>
+  <si>
+    <t>072920_XXX1_12_gWAT</t>
+  </si>
+  <si>
+    <t>072920_XXX1_13_iBAT</t>
+  </si>
+  <si>
+    <t>072920_XXX1_14_SI</t>
+  </si>
+  <si>
+    <t>072920_XXX1_15_ears</t>
   </si>
 </sst>
 </file>
@@ -552,9 +552,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -609,49 +643,49 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
@@ -674,16 +708,16 @@
         <v>0.82282200000000005</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M2">
         <v>0.39700000000000002</v>
@@ -766,16 +800,16 @@
         <v>0.82169499999999995</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M3">
         <v>0.39</v>
@@ -858,16 +892,16 @@
         <v>0.85142499999999999</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M4">
         <v>0.38300000000000001</v>
@@ -950,16 +984,16 @@
         <v>0.84902999999999995</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M5">
         <v>0.39200000000000002</v>
@@ -1042,16 +1076,16 @@
         <v>0.85051500000000002</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M6">
         <v>0.379</v>
@@ -1134,16 +1168,16 @@
         <v>0.85089800000000004</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M7">
         <v>0.39700000000000002</v>
@@ -1226,16 +1260,16 @@
         <v>0.84644900000000001</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="J8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="M8">
         <v>0.39</v>
@@ -1318,16 +1352,16 @@
         <v>0.82896300000000001</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M9">
         <v>0.69799999999999995</v>
@@ -1410,16 +1444,16 @@
         <v>0.84622699999999995</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M10">
         <v>0.70599999999999996</v>
@@ -1502,16 +1536,16 @@
         <v>0.84307100000000001</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="K11" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M11">
         <v>0.72899999999999998</v>
@@ -1594,16 +1628,16 @@
         <v>0.84671200000000002</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="K12" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="M12">
         <v>0.71</v>
@@ -1686,16 +1720,16 @@
         <v>0.83541200000000004</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="L13" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="M13">
         <v>0.65500000000000003</v>
@@ -1778,16 +1812,16 @@
         <v>0.84702599999999995</v>
       </c>
       <c r="I14" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="J14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="L14" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="M14">
         <v>0.66200000000000003</v>
@@ -1870,16 +1904,16 @@
         <v>0.83277299999999999</v>
       </c>
       <c r="I15" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="J15" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="L15" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="M15">
         <v>0.66400000000000003</v>
@@ -1954,13 +1988,35 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -1972,54 +2028,54 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2081,7 +2137,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2143,7 +2199,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2205,7 +2261,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2267,7 +2323,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -2329,7 +2385,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -2391,7 +2447,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -2453,7 +2509,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2515,7 +2571,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2577,7 +2633,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -2639,7 +2695,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2701,7 +2757,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2763,7 +2819,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2825,7 +2881,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2894,18 +2950,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -2917,54 +2993,54 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3023,7 +3099,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3082,7 +3158,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3141,7 +3217,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3200,7 +3276,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -3259,7 +3335,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -3318,7 +3394,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -3377,7 +3453,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3436,7 +3512,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3495,7 +3571,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -3554,7 +3630,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -3613,7 +3689,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3672,7 +3748,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3731,7 +3807,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3797,15 +3873,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -3817,54 +3914,54 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3923,7 +4020,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3982,7 +4079,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>0</v>

</xml_diff>